<commit_message>
[FEAT] include qualitative final demo
</commit_message>
<xml_diff>
--- a/qualitative/data/suzie_zuzek/data.xlsx
+++ b/qualitative/data/suzie_zuzek/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doerlbh/Dropbox/Git/smithsonian/qualitative/data/suzie_zuzek/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED1D0AD-CED1-0448-87F4-0B0563444393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59587059-A1C8-C44A-A6AE-E713DBDCC622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="3300" windowWidth="28040" windowHeight="17440" xr2:uid="{011CBE45-62A7-FD4B-A8EB-1F4A1AD9D5FB}"/>
+    <workbookView xWindow="3720" yWindow="2460" windowWidth="28040" windowHeight="17440" xr2:uid="{011CBE45-62A7-FD4B-A8EB-1F4A1AD9D5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -687,11 +687,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E815ABA8-D4BA-DB4C-9F83-2B5DDB929BDB}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>